<commit_message>
modify documents: README.md, API table.xlsx
</commit_message>
<xml_diff>
--- a/API table.xlsx
+++ b/API table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chang\Desktop\sparta\hanghae99\hanghae99-miniproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5F0B37-0F80-4FB8-BA4B-5CBF387C48D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D122A7A-3095-4524-B403-901C4ED52E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{552DEF19-3B23-4D56-8612-7A6C4AAE977F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>기능</t>
   </si>
@@ -64,117 +64,126 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>POST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ID 중복 검사</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중복시-{'msg':'이미 존재하는 아이디입니다.'}
-중복이 아닐 시-{'msg':'이미 존재하는 아이디입니다.'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/login</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인 성공시 - {'msg':'성공적으로 로그인 되었습니다.'}
-로그인 실패시 - {'msg':'아이디/비밀번호가 일치하지 않습니다.'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/signup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'id':login_user_id, 'pw'login_:user_pw}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'id':sp_user_id, 'pw':sp_user_pw}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'id':sp_user_id}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'msg':'회원가입이 완료되었습니다.'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>첫화면(메인 페이지)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천 맛집 리스트 로드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/recommend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천 맛집 리스트 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 로드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/idCheckup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천 맛집 리스트 보여주기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/recommend/postRecommendation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'region':region, 'res_name':res_name, 'url':url, 'description':description}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'msg':'성공적으로 게시되었습니다.'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/recommend/reviews</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/recommend/postReview</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성된 댓글 화면에 표시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'msg':'성공적으로 작성되었습니다.'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'id':user_id, comment':comment, 'star':star}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 페이지 로드(로그인 후)</t>
+    <t>/sign_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 성공시 - {'result': 'success', 'token': token}}
+로그인 실패시 - {'result': 'fail', 'msg': '아이디/비밀번호가 일치하지 않습니다.'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sign_up/save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인/회원가입 화면(첫 화면)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'result': 'success'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'username': username_receive, 'password': password_hash}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'username': username_receive, 'password': pw_hash}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디 중복 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/sign_up/check_dup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'username': username_receive}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'result': 'success', 'exists': exists}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ "url_link": url_link_receive,
+  "store_name": store_name_receive,
+  "location": location_receive,
+  "description": description_receive }</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'result': 'success', 'msg': '등록 완료!!'}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛집 등록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">맛집 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛집 화면에 표시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛집 상세 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/detail/&lt;keyword&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터베이스에서 맛집 정보를 가져옴
+{'store_name' : keyword}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/restaurantslist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록된 맛집 전체 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터베이스에서 받아온 맛집 정보를 클라이언트 단으로 전송
+return render_template("detail.html", matjip=matjip)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터베이스에서 받아온 정보를 클라이언트 단으로 전송
+return render_template('restaurantslist.html', matjiplist=matjip_list, current_time=d_today)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맛집 정보를 데이터베이스에서 받아옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -221,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -231,46 +240,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFDDDDDD"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FFDDDDDD"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFDDDDDD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFDDDDDD"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFDDDDDD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -280,7 +259,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -290,13 +269,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,23 +601,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0860AE15-1E96-47F6-94AF-A2413D4A628C}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.796875" customWidth="1"/>
     <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55" customWidth="1"/>
+    <col min="4" max="4" width="62.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -641,144 +629,180 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="D9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>